<commit_message>
Commit requerido por el sistema
</commit_message>
<xml_diff>
--- a/Archivos Excel/Credenciales - Portales.xlsx
+++ b/Archivos Excel/Credenciales - Portales.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\CapacitacionDesarrollo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\CapacitacionDesarrollo\Archivos Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45145810-D94F-4404-A004-CE74AC9A7A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27494B88-DD83-461C-9367-8AF821BEBF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{C30447A1-1B82-468F-95A4-B687C3F712A1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="47">
   <si>
     <t>Rubro</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>Intermex202201</t>
+  </si>
+  <si>
+    <t>Intermex.2022&amp;</t>
   </si>
 </sst>
 </file>
@@ -536,7 +539,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +586,7 @@
         <v>20</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Actualizancion de credenciasles en el archivo de portales crendeciales
</commit_message>
<xml_diff>
--- a/Archivos Excel/Credenciales - Portales.xlsx
+++ b/Archivos Excel/Credenciales - Portales.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\CapacitacionDesarrollo\Archivos Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\CapacitacionDesarrollo\Archivos Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27494B88-DD83-461C-9367-8AF821BEBF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E38733-D603-415A-AE29-9581316EC58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{C30447A1-1B82-468F-95A4-B687C3F712A1}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$F$23</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -144,9 +142,6 @@
     <t>P3632_1</t>
   </si>
   <si>
-    <t>HEB202201</t>
-  </si>
-  <si>
     <t>https://proveedores.liverpool.com.mx/irj/portal</t>
   </si>
   <si>
@@ -171,13 +166,16 @@
     <t>dist-intermex</t>
   </si>
   <si>
-    <t>Intermex.1123</t>
-  </si>
-  <si>
     <t>Intermex202201</t>
   </si>
   <si>
     <t>Intermex.2022&amp;</t>
+  </si>
+  <si>
+    <t>HEB202202</t>
+  </si>
+  <si>
+    <t>15%&amp;amp;Mar.22</t>
   </si>
 </sst>
 </file>
@@ -535,11 +533,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90EB8524-2A96-4355-9E6C-C92FB5BDEC40}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +571,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -586,10 +585,10 @@
         <v>20</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -606,7 +605,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -620,10 +619,10 @@
         <v>600787</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -640,7 +639,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -654,10 +653,10 @@
         <v>34</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -665,13 +664,13 @@
         <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -682,16 +681,16 @@
         <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -716,16 +715,16 @@
         <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -739,10 +738,10 @@
         <v>600787</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -759,7 +758,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -773,10 +772,10 @@
         <v>34</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -793,7 +792,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -801,16 +800,16 @@
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -830,7 +829,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -847,7 +846,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -861,10 +860,10 @@
         <v>34</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -881,7 +880,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -898,7 +897,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
@@ -912,10 +911,10 @@
         <v>600787</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
@@ -940,17 +939,23 @@
         <v>15</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="E23" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F23" xr:uid="{90EB8524-2A96-4355-9E6C-C92FB5BDEC40}"/>
+  <autoFilter ref="A1:F23" xr:uid="{90EB8524-2A96-4355-9E6C-C92FB5BDEC40}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Chedraui"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agrega un query en Folios para el paso de todos los registros que esten en Descarga Incompleta, Pagadas y Descarga Incompleta Pagadas a la tabla de Pendientes Walmart
</commit_message>
<xml_diff>
--- a/Archivos Excel/Credenciales - Portales.xlsx
+++ b/Archivos Excel/Credenciales - Portales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\CapacitacionDesarrollo\Archivos Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F11A6AD-0C64-48BF-9474-9F20C91AA901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EA9FC7D-8764-4D9F-A7DD-817B1600B09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{C30447A1-1B82-468F-95A4-B687C3F712A1}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$F$23</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="48">
   <si>
     <t>Rubro</t>
   </si>
@@ -176,6 +177,9 @@
   </si>
   <si>
     <t>Intermex.2022&amp;2</t>
+  </si>
+  <si>
+    <t>p005321896</t>
   </si>
 </sst>
 </file>
@@ -548,7 +552,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +684,7 @@
         <v>35</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cambio de contraseña de HEB
</commit_message>
<xml_diff>
--- a/Archivos Excel/Credenciales - Portales.xlsx
+++ b/Archivos Excel/Credenciales - Portales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\CapacitacionDesarrollo\Archivos Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EA9FC7D-8764-4D9F-A7DD-817B1600B09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB80C3AE-5B6F-4627-99E3-2A3DA5537177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{C30447A1-1B82-468F-95A4-B687C3F712A1}"/>
   </bookViews>
@@ -164,22 +164,22 @@
     <t>dist-intermex</t>
   </si>
   <si>
-    <t>HEB032022</t>
-  </si>
-  <si>
     <t>Intermex202204</t>
   </si>
   <si>
     <t>Enero$14572</t>
   </si>
   <si>
-    <t>18%&amp;Abr.22</t>
-  </si>
-  <si>
     <t>Intermex.2022&amp;2</t>
   </si>
   <si>
     <t>p005321896</t>
+  </si>
+  <si>
+    <t>18%&amp;Abr.23</t>
+  </si>
+  <si>
+    <t>Intermex.0522</t>
   </si>
 </sst>
 </file>
@@ -223,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -232,6 +232,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -548,11 +551,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90EB8524-2A96-4355-9E6C-C92FB5BDEC40}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,7 +602,7 @@
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -633,7 +636,7 @@
         <v>600787</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -667,7 +670,7 @@
         <v>33</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -684,7 +687,7 @@
         <v>35</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -718,7 +721,7 @@
         <v>18</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -735,7 +738,7 @@
         <v>41</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F10" s="3"/>
     </row>
@@ -752,8 +755,8 @@
       <c r="D11" s="2">
         <v>600787</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>43</v>
+      <c r="E11" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -787,7 +790,7 @@
         <v>33</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -875,7 +878,7 @@
         <v>33</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -926,7 +929,7 @@
         <v>600787</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -960,8 +963,11 @@
         <v>41</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>45</v>
-      </c>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F23" xr:uid="{90EB8524-2A96-4355-9E6C-C92FB5BDEC40}"/>

</xml_diff>